<commit_message>
Criei mais dois arquivos html, assess_iso, assess_prop, atualizei os arquivos views.py, models.py, forms.py, urls.py, assessments.html, assess_cis.html e assess_nist.html
</commit_message>
<xml_diff>
--- a/media/framework_generico.xlsx
+++ b/media/framework_generico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://castlebr.sharepoint.com/sites/ProjetoCyberGuard/Documentos Compartilhados/General/02. Modelo Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{1BDAFBE4-B95A-4973-8553-7B83167329B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{240904A2-81DA-451A-9E49-58DC2AC5C126}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6ACED00-D5F8-4126-847E-D267FCA48C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{158CF3EA-4292-473D-8901-1209D792411F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Id Controle*</t>
   </si>
@@ -57,13 +57,25 @@
   </si>
   <si>
     <t>Informações Adicionais</t>
+  </si>
+  <si>
+    <t>Resultado (Css)</t>
+  </si>
+  <si>
+    <t>Resultado (Cl.)</t>
+  </si>
+  <si>
+    <t>Comentários</t>
+  </si>
+  <si>
+    <t>Meta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,26 +486,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1033A23-0FC3-448C-BCD0-793E165D11C8}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" hidden="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,6 +528,18 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -533,15 +559,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9FBB26C75ACCD428F582D176A1C0D8D" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="9e1b15a4ed351b5b7a0ddbdab7557901">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="778279ca-e34c-4359-ba42-be3d0eb65c6e" xmlns:ns3="c0f88865-b3d4-4bff-80c2-a72bc0e13a31" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12f7ef5ea66dc786e6528c9402bf5a44" ns2:_="" ns3:_="">
     <xsd:import namespace="778279ca-e34c-4359-ba42-be3d0eb65c6e"/>
@@ -742,46 +759,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98A5B40B-813A-4E1A-BF3D-44AD6F2DB28B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c0f88865-b3d4-4bff-80c2-a72bc0e13a31"/>
-    <ds:schemaRef ds:uri="778279ca-e34c-4359-ba42-be3d0eb65c6e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98A5B40B-813A-4E1A-BF3D-44AD6F2DB28B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E9E460-7ADC-474A-A10C-61777A480F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F696E79-36DF-449B-9B6C-50AA79B9BD99}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F696E79-36DF-449B-9B6C-50AA79B9BD99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="778279ca-e34c-4359-ba42-be3d0eb65c6e"/>
-    <ds:schemaRef ds:uri="c0f88865-b3d4-4bff-80c2-a72bc0e13a31"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E9E460-7ADC-474A-A10C-61777A480F3E}"/>
 </file>
</xml_diff>